<commit_message>
add REST API 스펙 정의 & database design & 작업환경 등
</commit_message>
<xml_diff>
--- a/팀프로젝트/요구사항 명세서 (Requirements Specification).xlsx
+++ b/팀프로젝트/요구사항 명세서 (Requirements Specification).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\82108\OneDrive\바탕 화면\코드프레소\YC-Tech-Academy-TeamProject\팀프로젝트\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDAA728-3F29-4F3F-9D8B-AF7F7CFC87C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D97A5D6-F021-4558-944F-0D152C896E68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="49">
   <si>
     <t>RQ-ID</t>
   </si>
@@ -1168,6 +1168,13 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
+    <t>RQ-0008</t>
+  </si>
+  <si>
+    <t>회원 저장</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -1181,6 +1188,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> / </t>
     </r>
@@ -1197,6 +1205,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> / </t>
     </r>
@@ -1213,6 +1222,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> / </t>
     </r>
@@ -1229,6 +1239,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> / </t>
     </r>
@@ -1245,6 +1256,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> / </t>
     </r>
@@ -1261,6 +1273,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> / </t>
     </r>
@@ -1277,14 +1290,16 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> / &lt;</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
-        <rFont val="Arial Unicode MS"/>
-        <family val="2"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
       </rPr>
       <t>저장</t>
     </r>
@@ -1292,6 +1307,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t>&gt;
 [</t>
@@ -1309,6 +1325,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">] </t>
     </r>
@@ -1325,6 +1342,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 [</t>
@@ -1342,6 +1360,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">] </t>
     </r>
@@ -1358,6 +1377,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 [</t>
@@ -1375,6 +1395,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">] </t>
     </r>
@@ -1391,6 +1412,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1407,6 +1429,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1423,6 +1446,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 [</t>
@@ -1440,6 +1464,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">] </t>
     </r>
@@ -1456,6 +1481,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t>/</t>
     </r>
@@ -1472,6 +1498,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 [</t>
@@ -1489,6 +1516,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">] </t>
     </r>
@@ -1506,6 +1534,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t>[</t>
     </r>
@@ -1522,6 +1551,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">] </t>
     </r>
@@ -1538,6 +1568,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1554,6 +1585,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1570,6 +1602,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1586,6 +1619,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 [</t>
@@ -1603,6 +1637,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">] </t>
     </r>
@@ -1619,6 +1654,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1635,6 +1671,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
@@ -1651,6 +1688,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t>-</t>
     </r>
@@ -1667,6 +1705,7 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Trebuchet MS"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">
 &lt;</t>
@@ -1674,17 +1713,275 @@
     <r>
       <rPr>
         <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>저장</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>저장</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>버튼</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>클릭</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>시</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>해당</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>일정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>저장</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>및</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>메인</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>화면으로</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Trebuchet MS"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>이동</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>RQ-0009</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>회원가입</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
       </rPr>
-      <t>저장</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Trebuchet MS"/>
-      </rPr>
-      <t xml:space="preserve">&gt; </t>
+      <t>화면</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원목록화면</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>회원 목록 조회</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>회원</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>정보를</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>저장한다</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
     </r>
     <r>
       <rPr>
@@ -1692,180 +1989,105 @@
         <rFont val="Arial Unicode MS"/>
         <family val="2"/>
       </rPr>
-      <t>저장</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>버튼</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Trebuchet MS"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>클릭</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Trebuchet MS"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>시</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Trebuchet MS"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>해당</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Trebuchet MS"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>일정</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Trebuchet MS"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
+      <t xml:space="preserve">
+</t>
     </r>
     <r>
       <rPr>
         <sz val="10"/>
         <rFont val="Arial Unicode MS"/>
-        <family val="2"/>
-      </rPr>
-      <t>저장</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Trebuchet MS"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>및</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Trebuchet MS"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>메인</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Trebuchet MS"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>화면으로</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Trebuchet MS"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="돋움"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>이동</t>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t xml:space="preserve">
+[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>이름</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>]
+[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>주소</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>]:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>도시</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>거리</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>우편번호</t>
     </r>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="맑은 고딕"/>
-        <family val="3"/>
-        <charset val="129"/>
-      </rPr>
-      <t>정지운</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial Unicode MS"/>
-        <family val="2"/>
-      </rPr>
-      <t>, 김현중</t>
-    </r>
+    <t xml:space="preserve">회원 목록을 조회한다.
+(회원의 이름과 주소 목록)
+[이름]
+[주소]:도시, 거리, 우편번호
+</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -1876,7 +2098,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="m/d"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1976,6 +2198,12 @@
       <family val="3"/>
       <charset val="129"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -2009,7 +2237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2114,6 +2342,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2435,8 +2669,8 @@
   </sheetPr>
   <dimension ref="A1:J82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2663,7 +2897,7 @@
       </c>
       <c r="J8" s="4"/>
     </row>
-    <row r="9" spans="1:10" ht="153">
+    <row r="9" spans="1:10" ht="157">
       <c r="A9" s="4"/>
       <c r="B9" s="32" t="s">
         <v>36</v>
@@ -2675,13 +2909,13 @@
         <v>38</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F9" s="9">
         <v>45204</v>
       </c>
-      <c r="G9" s="35" t="s">
-        <v>41</v>
+      <c r="G9" s="24" t="s">
+        <v>28</v>
       </c>
       <c r="H9" s="33" t="s">
         <v>18</v>
@@ -2691,28 +2925,60 @@
       </c>
       <c r="J9" s="4"/>
     </row>
-    <row r="10" spans="1:10" ht="13.5">
+    <row r="10" spans="1:10" ht="60.5">
       <c r="A10" s="4"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="B10" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="9">
+        <v>45204</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="I10" s="27" t="s">
+        <v>19</v>
+      </c>
       <c r="J10" s="4"/>
     </row>
-    <row r="11" spans="1:10" ht="13.5">
+    <row r="11" spans="1:10" ht="91">
       <c r="A11" s="4"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="B11" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="9">
+        <v>45204</v>
+      </c>
+      <c r="G11" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>19</v>
+      </c>
       <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10" ht="13.5">

</xml_diff>